<commit_message>
Updated to actual motor values
</commit_message>
<xml_diff>
--- a/mechanical/Mechanical/SOLIDWORKS/BOM.xlsx
+++ b/mechanical/Mechanical/SOLIDWORKS/BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ho Jin\Documents\GitHub\MSE312\mechanical\SOLIDWORKS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ho Jin\Documents\GitHub\MSE312\mechanical\Mechanical\SOLIDWORKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E759654C-F6ED-4EE9-8B43-79CCBC508439}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB802A6E-0666-46A5-B659-C20852E9F6CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5113E8A9-D0E6-4E6B-BEEB-5AB6B2B68602}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Part </t>
   </si>
@@ -74,9 +74,6 @@
     <t>Output Gear (60 teeth)</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/trinamic-motion-control-gmbh/QBL4208-100-04-025/4843440</t>
-  </si>
-  <si>
     <t>https://www.mcmaster.com/2664N468/</t>
   </si>
   <si>
@@ -99,6 +96,15 @@
   </si>
   <si>
     <t>1020 8020 Extrusion (10 cm) ($0.36 / cm)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/crouzet/82890001/3190319</t>
+  </si>
+  <si>
+    <t>Motor Controller</t>
+  </si>
+  <si>
+    <t>https://www.pololu.com/product/2991</t>
   </si>
 </sst>
 </file>
@@ -184,13 +190,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1514475</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>161221</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>18099</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -524,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{156A48FD-430D-4AC0-948A-E685387787CA}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +560,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -563,7 +569,7 @@
         <v>8.4600000000000009</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D10" si="0">C2*B2</f>
+        <f t="shared" ref="D2:D11" si="0">C2*B2</f>
         <v>8.4600000000000009</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -572,7 +578,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -590,7 +596,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -603,12 +609,12 @@
         <v>64.34</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -621,7 +627,7 @@
         <v>26.32</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -668,53 +674,70 @@
         <v>174.61</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="0"/>
-        <v>174.61</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>180.98</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>29.95</v>
+      </c>
+      <c r="D9" s="1">
+        <f>C9</f>
+        <v>29.95</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1">
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
         <v>19.329999999999998</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D10" s="1">
         <f t="shared" si="0"/>
         <v>19.329999999999998</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1">
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
         <v>38.549999999999997</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D11" s="1">
         <f t="shared" si="0"/>
         <v>38.549999999999997</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D20" s="1">
-        <f>SUM(D2:D10)</f>
-        <v>424.55</v>
+      <c r="E11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="1">
+        <f>SUM(D2:D11)</f>
+        <v>460.86999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>